<commit_message>
mod foo_helper.py to use less disk space.
</commit_message>
<xml_diff>
--- a/food_data.xlsx
+++ b/food_data.xlsx
@@ -15,7 +15,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>Unnamed: 0.1</t>
+  </si>
   <si>
     <t>种类</t>
   </si>
@@ -516,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,7 +530,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,159 +552,207 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s"/>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s"/>
-      <c r="E2" t="n">
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s"/>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s"/>
+      <c r="G2" t="n">
         <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
       </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s"/>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s"/>
-      <c r="E3" t="n">
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s"/>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s"/>
+      <c r="G3" t="n">
         <v>15</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s"/>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s"/>
-      <c r="E4" t="n">
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s"/>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s"/>
+      <c r="G4" t="n">
         <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
       </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s"/>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s"/>
-      <c r="E5" t="n">
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s"/>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s"/>
+      <c r="G5" t="n">
         <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>23</v>
       </c>
       <c r="H5" t="s">
         <v>24</v>
       </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s"/>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s"/>
-      <c r="E6" t="n">
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s"/>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s"/>
+      <c r="G6" t="n">
         <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
       </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s"/>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s"/>
-      <c r="E7" t="n">
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s"/>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s"/>
+      <c r="G7" t="n">
         <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
       </c>
       <c r="H7" t="s">
         <v>33</v>
       </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s"/>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" t="s"/>
-      <c r="E8" t="n">
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s"/>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s"/>
+      <c r="G8" t="n">
         <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>